<commit_message>
added more strings to the mapping excel
</commit_message>
<xml_diff>
--- a/resources/tutkinto-mapping.xlsx
+++ b/resources/tutkinto-mapping.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\workspace\lupapiste\src\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="255">
   <si>
     <t>a</t>
   </si>
@@ -514,6 +519,273 @@
   </si>
   <si>
     <t>LVI-teknikko</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri yamk</t>
+  </si>
+  <si>
+    <t>teknikko,talonrakennustekniikka</t>
+  </si>
+  <si>
+    <t>amk ins</t>
+  </si>
+  <si>
+    <t>diplomingenjör</t>
+  </si>
+  <si>
+    <t>talonrakennustekniikka</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri (asiantuntija)</t>
+  </si>
+  <si>
+    <t>arkkitehdin tutkinto</t>
+  </si>
+  <si>
+    <t>insinööri (amk) rakennustekniikan koulutusohjelma</t>
+  </si>
+  <si>
+    <t>lvi- asentaja</t>
+  </si>
+  <si>
+    <t>insinööri (yamk)</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri (amk)</t>
+  </si>
+  <si>
+    <t>di (rak)</t>
+  </si>
+  <si>
+    <t>ri, ra(amk)</t>
+  </si>
+  <si>
+    <t>ins, (amk). rakennustekniikka</t>
+  </si>
+  <si>
+    <t>lvi-ins.amk (1996)</t>
+  </si>
+  <si>
+    <t>lvi-tekn</t>
+  </si>
+  <si>
+    <t>dipl.ins</t>
+  </si>
+  <si>
+    <t>rakennusmestari amk</t>
+  </si>
+  <si>
+    <t>ins.amk rakennetekniikka</t>
+  </si>
+  <si>
+    <t>lvi-insinööri amk</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri(amk)</t>
+  </si>
+  <si>
+    <t>lvi- ja energiatekniikan insinööri (amk)</t>
+  </si>
+  <si>
+    <t>rakennusarkkitehti (amk)</t>
+  </si>
+  <si>
+    <t>lvi teknikko</t>
+  </si>
+  <si>
+    <t>rakennus insinööri (amk)</t>
+  </si>
+  <si>
+    <t>talonrakennus teknikko</t>
+  </si>
+  <si>
+    <t>insinööri, talonrakennustekniikka</t>
+  </si>
+  <si>
+    <t>lvi ins (amk)</t>
+  </si>
+  <si>
+    <t>insinööri (rakennustekniikka), constructing architect</t>
+  </si>
+  <si>
+    <t>rakennustekniikan perustutkinto, insinööri (amk)</t>
+  </si>
+  <si>
+    <t>talonrakennusmestari</t>
+  </si>
+  <si>
+    <t>bachelor's degree in architecture, rakennusarkkitehti</t>
+  </si>
+  <si>
+    <t>ri-amk</t>
+  </si>
+  <si>
+    <t>insinööri (amk), rakennetekniikka</t>
+  </si>
+  <si>
+    <t>amk ri</t>
+  </si>
+  <si>
+    <t>rak. ins. (amk), talonrakennustekniikan koulutusohjelma</t>
+  </si>
+  <si>
+    <t>ra, arkkitehti</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri ri amk</t>
+  </si>
+  <si>
+    <t>insinööri (amk), talonrakennustekniikka</t>
+  </si>
+  <si>
+    <t>rakennusinsihööri</t>
+  </si>
+  <si>
+    <t>rkm ja lvi-insinööri amk</t>
+  </si>
+  <si>
+    <t>arkkitehti di</t>
+  </si>
+  <si>
+    <t>diblomi-insinööri</t>
+  </si>
+  <si>
+    <t>rak. ins.</t>
+  </si>
+  <si>
+    <t>ri. amkk</t>
+  </si>
+  <si>
+    <t>rakennusarkkitehti, amk</t>
+  </si>
+  <si>
+    <t>ra/arkkkitehti</t>
+  </si>
+  <si>
+    <t>taiteen maisteri,sis.arkkit.</t>
+  </si>
+  <si>
+    <t>rak ark</t>
+  </si>
+  <si>
+    <t>yhdyskuntatekniikan insinööri</t>
+  </si>
+  <si>
+    <t>ri amk, ra,</t>
+  </si>
+  <si>
+    <t>suunnitteluassistentti</t>
+  </si>
+  <si>
+    <t>arkkitehtti-yo</t>
+  </si>
+  <si>
+    <t>rkm talonrakennusteknikko</t>
+  </si>
+  <si>
+    <t>arkkitehti ttkk</t>
+  </si>
+  <si>
+    <t>ympäristöinsinööri</t>
+  </si>
+  <si>
+    <t>tkk (arkkitehtuuri)</t>
+  </si>
+  <si>
+    <t>kone- ja tuotantotekniikan insinööri</t>
+  </si>
+  <si>
+    <t>rak. osaston yhdyskuntatekn. ins.</t>
+  </si>
+  <si>
+    <t>putkiasentaja</t>
+  </si>
+  <si>
+    <t>rakennusrestauroinnin artesaani</t>
+  </si>
+  <si>
+    <t>koneautomaatio</t>
+  </si>
+  <si>
+    <t>puuseppä</t>
+  </si>
+  <si>
+    <t>rkm .tie vesirak .talonrak .hitsaustek.</t>
+  </si>
+  <si>
+    <t>rkm, tampereen tekninen koulu / tien- ja vesirakennus</t>
+  </si>
+  <si>
+    <t>opisto</t>
+  </si>
+  <si>
+    <t>amk vallilan talonrakennuslinja</t>
+  </si>
+  <si>
+    <t>isännöitsijäammattitutkinto</t>
+  </si>
+  <si>
+    <t>insinööri (puutekniikka)</t>
+  </si>
+  <si>
+    <t>suunnitteluavustaja</t>
+  </si>
+  <si>
+    <t>rak.arkk</t>
+  </si>
+  <si>
+    <t>raksa inssi</t>
+  </si>
+  <si>
+    <t>rakennusinsinööri /talonrakennus</t>
+  </si>
+  <si>
+    <t>byggmästare</t>
+  </si>
+  <si>
+    <t>talotekniikan insinööri (amk)</t>
+  </si>
+  <si>
+    <t>rak. ins. amk (talonrakennustekniikka)</t>
+  </si>
+  <si>
+    <t>s1 sähköturvallisuus tutkinto</t>
+  </si>
+  <si>
+    <t>rak di</t>
+  </si>
+  <si>
+    <t>iat</t>
+  </si>
+  <si>
+    <t>insinööri yamk</t>
+  </si>
+  <si>
+    <t>lvi</t>
+  </si>
+  <si>
+    <t>di, rakenne- ja rakennustuotantotekniikka</t>
+  </si>
+  <si>
+    <t>ri (yamk)</t>
+  </si>
+  <si>
+    <t>ins (amk)</t>
+  </si>
+  <si>
+    <t>arkkitehti, di (talonrak.)</t>
+  </si>
+  <si>
+    <t>rakennusinsinöörii</t>
+  </si>
+  <si>
+    <t>suunnitteluhortonomi amk</t>
+  </si>
+  <si>
+    <t>insinööri, yhdyskuntatekniikka</t>
+  </si>
+  <si>
+    <t>rakennusalan työnjohdon koulutus (amk)</t>
   </si>
 </sst>
 </file>
@@ -560,6 +832,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -608,7 +883,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -643,7 +918,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -852,15 +1127,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:B255"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -890,55 +1165,55 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -946,31 +1221,31 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
         <v>102</v>
@@ -978,15 +1253,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -994,7 +1269,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -1002,7 +1277,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -1010,7 +1285,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -1018,103 +1293,103 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>161</v>
@@ -1122,119 +1397,119 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>247</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>208</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
         <v>161</v>
@@ -1242,7 +1517,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
         <v>161</v>
@@ -1250,7 +1525,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
         <v>161</v>
@@ -1258,623 +1533,623 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>249</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>245</v>
       </c>
       <c r="B63" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="B65" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>194</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>253</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="B70" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>179</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>244</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>227</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>246</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B92" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B97" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B99" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>187</v>
       </c>
       <c r="B101" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="B102" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B105" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="B108" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>231</v>
       </c>
       <c r="B110" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="B111" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="B119" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="B120" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="B121" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="B123" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="B124" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="B125" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>216</v>
       </c>
       <c r="B126" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
         <v>107</v>
@@ -1882,79 +2157,79 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="B128" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>236</v>
       </c>
       <c r="B132" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="B133" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="B134" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>243</v>
       </c>
       <c r="B135" t="s">
-        <v>114</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B136" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>209</v>
       </c>
       <c r="B137" t="s">
         <v>107</v>
@@ -1962,175 +2237,175 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="B138" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="B139" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>237</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="B142" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>241</v>
       </c>
       <c r="B143" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>251</v>
       </c>
       <c r="B144" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B145" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="B146" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>201</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="B148" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B150" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="B151" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="B152" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="B153" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="B154" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="B155" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B158" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="B159" t="s">
         <v>161</v>
@@ -2138,31 +2413,31 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
       <c r="B160" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="B162" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="B163" t="s">
         <v>161</v>
@@ -2170,9 +2445,737 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>102</v>
+      </c>
+      <c r="B164" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>103</v>
+      </c>
+      <c r="B165" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>211</v>
+      </c>
+      <c r="B166" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>188</v>
+      </c>
+      <c r="B167" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>104</v>
+      </c>
+      <c r="B168" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>105</v>
+      </c>
+      <c r="B169" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>106</v>
+      </c>
+      <c r="B170" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>107</v>
+      </c>
+      <c r="B171" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>108</v>
+      </c>
+      <c r="B172" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>186</v>
+      </c>
+      <c r="B173" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>109</v>
+      </c>
+      <c r="B174" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>110</v>
+      </c>
+      <c r="B175" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>166</v>
+      </c>
+      <c r="B176" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>111</v>
+      </c>
+      <c r="B177" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>112</v>
+      </c>
+      <c r="B179" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>113</v>
+      </c>
+      <c r="B180" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>114</v>
+      </c>
+      <c r="B181" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>183</v>
+      </c>
+      <c r="B182" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>115</v>
+      </c>
+      <c r="B183" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>116</v>
+      </c>
+      <c r="B184" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>226</v>
+      </c>
+      <c r="B185" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>196</v>
+      </c>
+      <c r="B186" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>117</v>
+      </c>
+      <c r="B187" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>118</v>
+      </c>
+      <c r="B188" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>119</v>
+      </c>
+      <c r="B189" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>120</v>
+      </c>
+      <c r="B190" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>121</v>
+      </c>
+      <c r="B191" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>122</v>
+      </c>
+      <c r="B192" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>123</v>
+      </c>
+      <c r="B193" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>124</v>
+      </c>
+      <c r="B194" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>125</v>
+      </c>
+      <c r="B195" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>198</v>
+      </c>
+      <c r="B196" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>126</v>
+      </c>
+      <c r="B197" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>127</v>
+      </c>
+      <c r="B198" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>128</v>
+      </c>
+      <c r="B199" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>129</v>
+      </c>
+      <c r="B200" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>130</v>
+      </c>
+      <c r="B201" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>210</v>
+      </c>
+      <c r="B202" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>248</v>
+      </c>
+      <c r="B203" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>131</v>
+      </c>
+      <c r="B204" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>132</v>
+      </c>
+      <c r="B205" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>133</v>
+      </c>
+      <c r="B206" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>134</v>
+      </c>
+      <c r="B207" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>135</v>
+      </c>
+      <c r="B208" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>136</v>
+      </c>
+      <c r="B209" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>206</v>
+      </c>
+      <c r="B210" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>137</v>
+      </c>
+      <c r="B211" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>219</v>
+      </c>
+      <c r="B212" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>138</v>
+      </c>
+      <c r="B213" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>139</v>
+      </c>
+      <c r="B214" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>229</v>
+      </c>
+      <c r="B215" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>230</v>
+      </c>
+      <c r="B216" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>242</v>
+      </c>
+      <c r="B217" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>140</v>
+      </c>
+      <c r="B218" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>141</v>
+      </c>
+      <c r="B219" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>217</v>
+      </c>
+      <c r="B220" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>235</v>
+      </c>
+      <c r="B221" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>252</v>
+      </c>
+      <c r="B222" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>213</v>
+      </c>
+      <c r="B223" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>142</v>
+      </c>
+      <c r="B224" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>143</v>
+      </c>
+      <c r="B225" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>196</v>
+      </c>
+      <c r="B226" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>144</v>
+      </c>
+      <c r="B227" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>192</v>
+      </c>
+      <c r="B228" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>204</v>
+      </c>
+      <c r="B229" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>145</v>
+      </c>
+      <c r="B230" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>191</v>
+      </c>
+      <c r="B231" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>167</v>
+      </c>
+      <c r="B232" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>170</v>
+      </c>
+      <c r="B233" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>146</v>
+      </c>
+      <c r="B234" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>147</v>
+      </c>
+      <c r="B235" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>148</v>
+      </c>
+      <c r="B236" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>240</v>
+      </c>
+      <c r="B237" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>149</v>
+      </c>
+      <c r="B238" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>150</v>
+      </c>
+      <c r="B239" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>151</v>
+      </c>
+      <c r="B240" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>152</v>
+      </c>
+      <c r="B241" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>153</v>
+      </c>
+      <c r="B242" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>154</v>
+      </c>
+      <c r="B243" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>155</v>
+      </c>
+      <c r="B244" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>156</v>
+      </c>
+      <c r="B245" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>157</v>
+      </c>
+      <c r="B246" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>222</v>
+      </c>
+      <c r="B247" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>158</v>
+      </c>
+      <c r="B248" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>159</v>
+      </c>
+      <c r="B249" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
         <v>160</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B250" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>158</v>
+      </c>
+      <c r="B251" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>159</v>
+      </c>
+      <c r="B252" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>215</v>
+      </c>
+      <c r="B253" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>221</v>
+      </c>
+      <c r="B254" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>160</v>
+      </c>
+      <c r="B255" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- not anymore matching the strings that have multiple degrees in them - changed "muu" values to "other" since we now have the other-key mechanism in use
</commit_message>
<xml_diff>
--- a/resources/tutkinto-mapping.xlsx
+++ b/resources/tutkinto-mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="232">
   <si>
     <t>a</t>
   </si>
@@ -41,9 +41,6 @@
     <t>ark</t>
   </si>
   <si>
-    <t>ark / ra</t>
-  </si>
-  <si>
     <t>ark yo</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>arkkitehti</t>
   </si>
   <si>
-    <t>arkkitehti / rakennusarkkitehti 1996</t>
-  </si>
-  <si>
     <t>arkkitehti amk</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>artesaanipuuseppä</t>
   </si>
   <si>
-    <t>cdhweufdgw</t>
-  </si>
-  <si>
     <t>di</t>
   </si>
   <si>
@@ -122,12 +113,6 @@
     <t>fm</t>
   </si>
   <si>
-    <t>gfhserhrma</t>
-  </si>
-  <si>
-    <t>htyhtyhyt</t>
-  </si>
-  <si>
     <t>ins</t>
   </si>
   <si>
@@ -161,15 +146,6 @@
     <t>insinööri, rakennustekniikka</t>
   </si>
   <si>
-    <t>jdcoqugf</t>
-  </si>
-  <si>
-    <t>jdvfhwvho</t>
-  </si>
-  <si>
-    <t>jonkinlainen</t>
-  </si>
-  <si>
     <t>kirvesmies</t>
   </si>
   <si>
@@ -179,12 +155,6 @@
     <t>koneinsinöörioppilas</t>
   </si>
   <si>
-    <t>ksöflkajsfl</t>
-  </si>
-  <si>
-    <t>laitoin itseni pääsuunnittelijaksi, koska nykyiselle päärakennukselle ei tehdä toimenpiteitä, haen vain käyttötarkoituksen muutiosta, rakennuslupahakemukseen laitan pääsuunnittelijan</t>
-  </si>
-  <si>
     <t>lvi asentaja</t>
   </si>
   <si>
@@ -248,12 +218,6 @@
     <t>ra</t>
   </si>
   <si>
-    <t>ra / ark</t>
-  </si>
-  <si>
-    <t>ra /rkm</t>
-  </si>
-  <si>
     <t>ra ark 584</t>
   </si>
   <si>
@@ -263,9 +227,6 @@
     <t>ra.arkk.</t>
   </si>
   <si>
-    <t>ra/ri</t>
-  </si>
-  <si>
     <t>rak. ins</t>
   </si>
   <si>
@@ -296,9 +257,6 @@
     <t>rak.ins.amk</t>
   </si>
   <si>
-    <t>rak.ins/rkm/lehtori</t>
-  </si>
-  <si>
     <t>rak.mest</t>
   </si>
   <si>
@@ -431,9 +389,6 @@
     <t>rkm (amk)</t>
   </si>
   <si>
-    <t>rkm ja ri</t>
-  </si>
-  <si>
     <t>rkm talonrakennus</t>
   </si>
   <si>
@@ -491,9 +446,6 @@
     <t>tekninen koulu</t>
   </si>
   <si>
-    <t>testi</t>
-  </si>
-  <si>
     <t>testitutkinto</t>
   </si>
   <si>
@@ -506,9 +458,6 @@
     <t>yo</t>
   </si>
   <si>
-    <t>muu</t>
-  </si>
-  <si>
     <t>arkkitehtiylioppilas</t>
   </si>
   <si>
@@ -557,9 +506,6 @@
     <t>di (rak)</t>
   </si>
   <si>
-    <t>ri, ra(amk)</t>
-  </si>
-  <si>
     <t>ins, (amk). rakennustekniikka</t>
   </si>
   <si>
@@ -629,9 +575,6 @@
     <t>rak. ins. (amk), talonrakennustekniikan koulutusohjelma</t>
   </si>
   <si>
-    <t>ra, arkkitehti</t>
-  </si>
-  <si>
     <t>rakennusinsinööri ri amk</t>
   </si>
   <si>
@@ -641,9 +584,6 @@
     <t>rakennusinsihööri</t>
   </si>
   <si>
-    <t>rkm ja lvi-insinööri amk</t>
-  </si>
-  <si>
     <t>arkkitehti di</t>
   </si>
   <si>
@@ -659,9 +599,6 @@
     <t>rakennusarkkitehti, amk</t>
   </si>
   <si>
-    <t>ra/arkkkitehti</t>
-  </si>
-  <si>
     <t>taiteen maisteri,sis.arkkit.</t>
   </si>
   <si>
@@ -671,18 +608,12 @@
     <t>yhdyskuntatekniikan insinööri</t>
   </si>
   <si>
-    <t>ri amk, ra,</t>
-  </si>
-  <si>
     <t>suunnitteluassistentti</t>
   </si>
   <si>
     <t>arkkitehtti-yo</t>
   </si>
   <si>
-    <t>rkm talonrakennusteknikko</t>
-  </si>
-  <si>
     <t>arkkitehti ttkk</t>
   </si>
   <si>
@@ -716,9 +647,6 @@
     <t>rkm, tampereen tekninen koulu / tien- ja vesirakennus</t>
   </si>
   <si>
-    <t>opisto</t>
-  </si>
-  <si>
     <t>amk vallilan talonrakennuslinja</t>
   </si>
   <si>
@@ -786,6 +714,9 @@
   </si>
   <si>
     <t>rakennusalan työnjohdon koulutus (amk)</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -1127,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B255"/>
+  <dimension ref="A1:B231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1160,15 +1091,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1176,23 +1107,23 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,47 +1147,47 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,23 +1195,23 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" t="s">
         <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1219,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,39 +1227,39 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,31 +1275,31 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>197</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1315,7 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,119 +1323,119 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>247</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
         <v>27</v>
-      </c>
-      <c r="B40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>208</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,919 +1443,919 @@
         <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>225</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>249</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>244</v>
+        <v>43</v>
       </c>
       <c r="B73" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="B74" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="B76" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B77" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B78" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>246</v>
+        <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B88" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>193</v>
+        <v>54</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B93" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="B94" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="B96" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B99" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="B101" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B103" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="B104" t="s">
-        <v>165</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
-        <v>165</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B107" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B108" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B109" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>231</v>
+        <v>69</v>
       </c>
       <c r="B110" t="s">
-        <v>161</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>71</v>
+        <v>193</v>
       </c>
       <c r="B111" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>225</v>
+        <v>70</v>
       </c>
       <c r="B112" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>228</v>
+        <v>71</v>
       </c>
       <c r="B113" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="B114" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B115" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>212</v>
+        <v>74</v>
       </c>
       <c r="B118" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B120" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B121" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B122" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>213</v>
       </c>
       <c r="B123" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>214</v>
       </c>
       <c r="B124" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="B125" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B126" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="B127" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>82</v>
+        <v>172</v>
       </c>
       <c r="B128" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="B129" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="B130" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B131" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>236</v>
+        <v>79</v>
       </c>
       <c r="B132" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B133" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B134" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>243</v>
+        <v>82</v>
       </c>
       <c r="B135" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="B136" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="B137" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="B138" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="B139" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B140" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>237</v>
+        <v>85</v>
       </c>
       <c r="B141" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>238</v>
+        <v>186</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>241</v>
+        <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>251</v>
+        <v>87</v>
       </c>
       <c r="B144" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="B145" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="B146" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B147" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="B148" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>254</v>
+        <v>90</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B150" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B151" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B152" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B153" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B154" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>224</v>
+        <v>95</v>
       </c>
       <c r="B155" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B156" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
       <c r="B157" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B158" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B160" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>205</v>
+        <v>99</v>
       </c>
       <c r="B161" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,95 +2363,95 @@
         <v>100</v>
       </c>
       <c r="B162" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B164" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B165" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B166" t="s">
-        <v>102</v>
+        <v>231</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B167" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B168" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B169" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B170" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B171" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B172" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="B173" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -2528,7 +2459,7 @@
         <v>109</v>
       </c>
       <c r="B174" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2536,175 +2467,175 @@
         <v>110</v>
       </c>
       <c r="B175" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="B176" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="B177" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="B178" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B179" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B180" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B181" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>183</v>
+        <v>116</v>
       </c>
       <c r="B182" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="B183" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="B184" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="B185" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="B186" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B187" t="s">
-        <v>117</v>
+        <v>231</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B188" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B189" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B190" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B191" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B192" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="B193" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="B194" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>125</v>
+        <v>218</v>
       </c>
       <c r="B195" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="B196" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,471 +2643,279 @@
         <v>126</v>
       </c>
       <c r="B197" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
       <c r="B198" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="B199" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>129</v>
+        <v>228</v>
       </c>
       <c r="B200" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="B201" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>210</v>
+        <v>127</v>
       </c>
       <c r="B202" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>248</v>
+        <v>128</v>
       </c>
       <c r="B203" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="B204" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B205" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="B206" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>134</v>
+        <v>185</v>
       </c>
       <c r="B207" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B208" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="B209" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>206</v>
+        <v>150</v>
       </c>
       <c r="B210" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B211" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>219</v>
+        <v>131</v>
       </c>
       <c r="B212" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B213" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B214" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B215" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="B216" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>242</v>
+        <v>135</v>
       </c>
       <c r="B217" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B218" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B219" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
       <c r="B220" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>235</v>
+        <v>139</v>
       </c>
       <c r="B221" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>252</v>
+        <v>140</v>
       </c>
       <c r="B222" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>213</v>
+        <v>141</v>
       </c>
       <c r="B223" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="B224" t="s">
-        <v>161</v>
+        <v>10</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B225" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
       <c r="B226" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B227" t="s">
-        <v>144</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="B228" t="s">
-        <v>144</v>
+        <v>231</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B229" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>145</v>
+        <v>198</v>
       </c>
       <c r="B230" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="B231" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>167</v>
-      </c>
-      <c r="B232" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>170</v>
-      </c>
-      <c r="B233" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>146</v>
-      </c>
-      <c r="B234" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>147</v>
-      </c>
-      <c r="B235" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>148</v>
-      </c>
-      <c r="B236" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>240</v>
-      </c>
-      <c r="B237" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>149</v>
-      </c>
-      <c r="B238" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>150</v>
-      </c>
-      <c r="B239" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>151</v>
-      </c>
-      <c r="B240" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>152</v>
-      </c>
-      <c r="B241" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>153</v>
-      </c>
-      <c r="B242" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>154</v>
-      </c>
-      <c r="B243" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>155</v>
-      </c>
-      <c r="B244" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>156</v>
-      </c>
-      <c r="B245" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>157</v>
-      </c>
-      <c r="B246" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>222</v>
-      </c>
-      <c r="B247" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>158</v>
-      </c>
-      <c r="B248" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>159</v>
-      </c>
-      <c r="B249" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>160</v>
-      </c>
-      <c r="B250" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>158</v>
-      </c>
-      <c r="B251" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>159</v>
-      </c>
-      <c r="B252" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>215</v>
-      </c>
-      <c r="B253" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>221</v>
-      </c>
-      <c r="B254" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>160</v>
-      </c>
-      <c r="B255" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added line for "other"
</commit_message>
<xml_diff>
--- a/resources/tutkinto-mapping.xlsx
+++ b/resources/tutkinto-mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="232">
   <si>
     <t>a</t>
   </si>
@@ -1058,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:B232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A230" sqref="A230"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>61</v>
+        <v>231</v>
       </c>
       <c r="B100" t="s">
         <v>231</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="B101" t="s">
         <v>231</v>
@@ -1880,39 +1880,39 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="B103" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B104" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B106" t="s">
         <v>88</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B107" t="s">
         <v>88</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
         <v>88</v>
@@ -1936,31 +1936,31 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B109" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B110" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="B111" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="B112" t="s">
         <v>88</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B113" t="s">
         <v>88</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>212</v>
+        <v>71</v>
       </c>
       <c r="B114" t="s">
         <v>88</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s">
         <v>88</v>
@@ -1992,7 +1992,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B116" t="s">
         <v>88</v>
@@ -2000,23 +2000,23 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="B117" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="B118" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>189</v>
+        <v>74</v>
       </c>
       <c r="B119" t="s">
         <v>93</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B120" t="s">
         <v>93</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B121" t="s">
         <v>93</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B122" t="s">
         <v>93</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>213</v>
+        <v>77</v>
       </c>
       <c r="B123" t="s">
         <v>93</v>
@@ -2056,15 +2056,15 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B124" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B125" t="s">
         <v>129</v>
@@ -2072,15 +2072,15 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B126" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>159</v>
+        <v>227</v>
       </c>
       <c r="B127" t="s">
         <v>93</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B128" t="s">
         <v>93</v>
@@ -2096,23 +2096,23 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>78</v>
+        <v>230</v>
       </c>
       <c r="B131" t="s">
         <v>100</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B132" t="s">
         <v>100</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B133" t="s">
         <v>100</v>
@@ -2136,15 +2136,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B134" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B135" t="s">
         <v>106</v>
@@ -2152,23 +2152,23 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>201</v>
+        <v>82</v>
       </c>
       <c r="B136" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="B137" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B138" t="s">
         <v>93</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="B139" t="s">
         <v>93</v>
@@ -2184,23 +2184,23 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="B140" t="s">
-        <v>231</v>
+        <v>93</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B141" t="s">
-        <v>93</v>
+        <v>231</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="B142" t="s">
         <v>93</v>
@@ -2208,31 +2208,31 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="B143" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B144" t="s">
-        <v>231</v>
+        <v>27</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B145" t="s">
-        <v>88</v>
+        <v>231</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B146" t="s">
         <v>88</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>191</v>
+        <v>89</v>
       </c>
       <c r="B147" t="s">
         <v>88</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B148" t="s">
         <v>88</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="B149" t="s">
         <v>88</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B150" t="s">
         <v>88</v>
@@ -2272,15 +2272,15 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B151" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B152" t="s">
         <v>93</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B153" t="s">
         <v>93</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>94</v>
       </c>
       <c r="B154" t="s">
         <v>93</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>95</v>
+        <v>168</v>
       </c>
       <c r="B155" t="s">
         <v>93</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B156" t="s">
         <v>93</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="B157" t="s">
         <v>93</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="B158" t="s">
         <v>93</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="B159" t="s">
         <v>93</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>93</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B161" t="s">
         <v>93</v>
@@ -2360,15 +2360,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B162" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="B163" t="s">
         <v>100</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="B164" t="s">
         <v>100</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B165" t="s">
         <v>100</v>
@@ -2392,39 +2392,39 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>203</v>
+        <v>102</v>
       </c>
       <c r="B166" t="s">
-        <v>231</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="B167" t="s">
-        <v>100</v>
+        <v>231</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="B168" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B169" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B170" t="s">
         <v>93</v>
@@ -2432,23 +2432,23 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B171" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B172" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B173" t="s">
         <v>93</v>
@@ -2456,15 +2456,15 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B174" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B175" t="s">
         <v>100</v>
@@ -2472,15 +2472,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B176" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="B177" t="s">
         <v>93</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
         <v>93</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B179" t="s">
         <v>93</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B180" t="s">
         <v>93</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B181" t="s">
         <v>93</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B182" t="s">
         <v>93</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="B183" t="s">
         <v>93</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="B184" t="s">
         <v>93</v>
@@ -2544,15 +2544,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>117</v>
+        <v>224</v>
       </c>
       <c r="B185" t="s">
-        <v>231</v>
+        <v>93</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B186" t="s">
         <v>231</v>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B187" t="s">
         <v>231</v>
@@ -2568,15 +2568,15 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B188" t="s">
-        <v>100</v>
+        <v>231</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B189" t="s">
         <v>100</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B190" t="s">
         <v>100</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B191" t="s">
         <v>100</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B192" t="s">
         <v>100</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="B193" t="s">
         <v>100</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B194" t="s">
         <v>100</v>
@@ -2624,23 +2624,23 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B195" t="s">
-        <v>231</v>
+        <v>100</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>125</v>
+        <v>218</v>
       </c>
       <c r="B196" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B197" t="s">
         <v>126</v>
@@ -2648,15 +2648,15 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>195</v>
+        <v>126</v>
       </c>
       <c r="B198" t="s">
-        <v>231</v>
+        <v>126</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B199" t="s">
         <v>231</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B200" t="s">
         <v>231</v>
@@ -2672,47 +2672,47 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="B201" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="B202" t="s">
-        <v>231</v>
+        <v>126</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B203" t="s">
-        <v>139</v>
+        <v>231</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B204" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
       <c r="B205" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="B206" t="s">
         <v>129</v>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B207" t="s">
         <v>129</v>
@@ -2728,15 +2728,15 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="B208" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="B209" t="s">
         <v>130</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B210" t="s">
         <v>130</v>
@@ -2752,15 +2752,15 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B211" t="s">
-        <v>231</v>
+        <v>130</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="B212" t="s">
         <v>231</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B213" t="s">
         <v>231</v>
@@ -2776,15 +2776,15 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B214" t="s">
-        <v>34</v>
+        <v>231</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>216</v>
+        <v>133</v>
       </c>
       <c r="B215" t="s">
         <v>34</v>
@@ -2792,63 +2792,63 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>134</v>
+        <v>216</v>
       </c>
       <c r="B216" t="s">
-        <v>231</v>
+        <v>34</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B217" t="s">
-        <v>34</v>
+        <v>231</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B218" t="s">
-        <v>231</v>
+        <v>34</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B219" t="s">
-        <v>93</v>
+        <v>231</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B220" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B221" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B222" t="s">
-        <v>231</v>
+        <v>139</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B223" t="s">
         <v>231</v>
@@ -2856,23 +2856,23 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="B224" t="s">
-        <v>10</v>
+        <v>231</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="B225" t="s">
-        <v>231</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B226" t="s">
         <v>231</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B227" t="s">
         <v>231</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B228" t="s">
         <v>231</v>
@@ -2896,15 +2896,15 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="B229" t="s">
-        <v>34</v>
+        <v>231</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B230" t="s">
         <v>34</v>
@@ -2912,9 +2912,17 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>198</v>
+      </c>
+      <c r="B231" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>144</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>231</v>
       </c>
     </row>

</xml_diff>